<commit_message>
Adicinado toda parte positiva e parcialmente negativa
</commit_message>
<xml_diff>
--- a/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTesteBDD.xlsx
+++ b/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTesteBDD.xlsx
@@ -3,25 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FE5BFBBB-AAE8-45D8-98E0-A0BA60579DF4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F4A71BDE-9DB8-483A-AA00-03B64A6D8A0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20760" windowHeight="11820" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20820" windowHeight="11820" activeTab="1" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O7"/>
+  <oleSize ref="A1:H7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -519,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F38C2-8A9E-4E31-AEC9-72957AEA4A35}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +615,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="2">
-        <v>123</v>
+        <v>1234</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
@@ -661,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C03071B-E623-4E76-9706-B3CDEEE6E2A0}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adicionado todas funcoes basicas positiva e negativa
</commit_message>
<xml_diff>
--- a/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTesteBDD.xlsx
+++ b/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTesteBDD.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F4A71BDE-9DB8-483A-AA00-03B64A6D8A0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{36A5CF91-783C-4714-B969-0E3F7F9C723C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20820" windowHeight="11820" activeTab="1" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20910" windowHeight="11820" activeTab="1" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H7"/>
+  <oleSize ref="A1:L7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Nome Caso de Teste</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Mesa</t>
+  </si>
+  <si>
+    <t>usertest99</t>
   </si>
 </sst>
 </file>
@@ -190,12 +193,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -514,7 +520,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +571,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>15</v>
@@ -653,10 +659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C03071B-E623-4E76-9706-B3CDEEE6E2A0}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,6 +694,9 @@
         <v>31</v>
       </c>
     </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Alteraçoes em alguns asserts e adiciona report e 1 cenario
</commit_message>
<xml_diff>
--- a/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTesteBDD.xlsx
+++ b/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTesteBDD.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{36A5CF91-783C-4714-B969-0E3F7F9C723C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{377C505F-8721-4BC4-A24F-045511ED2028}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20910" windowHeight="11820" activeTab="1" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="20940" windowHeight="11820" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L7"/>
+  <oleSize ref="A1:N7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Nome Caso de Teste</t>
   </si>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F38C2-8A9E-4E31-AEC9-72957AEA4A35}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,10 +618,10 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1234</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
@@ -661,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C03071B-E623-4E76-9706-B3CDEEE6E2A0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Alterações do Report e pequenas alterações
</commit_message>
<xml_diff>
--- a/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTesteBDD.xlsx
+++ b/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTesteBDD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{377C505F-8721-4BC4-A24F-045511ED2028}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A947C0F7-8157-4BB1-A09E-A78ADFDE2C59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20940" windowHeight="11820" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20970" windowHeight="11820" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
     <t>Mesa</t>
   </si>
   <si>
-    <t>usertest99</t>
+    <t>usertest206</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adicinado Manager e feitas as devidas alterações
</commit_message>
<xml_diff>
--- a/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTesteBDD.xlsx
+++ b/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTesteBDD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A947C0F7-8157-4BB1-A09E-A78ADFDE2C59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5C7FCB80-23B9-4CC0-BA89-5857371D9DD4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20970" windowHeight="11820" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21000" windowHeight="11820" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
     <t>Mesa</t>
   </si>
   <si>
-    <t>usertest206</t>
+    <t>usertest208</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>